<commit_message>
add bảng so sánh
</commit_message>
<xml_diff>
--- a/Bangsosanh.xlsx
+++ b/Bangsosanh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocbinh/Documents/Lập trình mạng/Elearning_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocbinh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91E62421-051E-BE40-9BD7-7EB46DCD1616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBC079D-2C33-DD49-B149-A15FBDCE23E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{545EF46E-B425-7346-84DE-FF384B7C3F17}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{545EF46E-B425-7346-84DE-FF384B7C3F17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Python (asyncio)</t>
   </si>
@@ -79,9 +79,6 @@
     <t>async/await</t>
   </si>
   <si>
-    <t>OpenSwoole</t>
-  </si>
-  <si>
     <t>Mô hình async</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>Hiệu suất cao nhất</t>
   </si>
   <si>
-    <t>PHP dev dễ chuyển</t>
-  </si>
-  <si>
     <t>GIL (CPU-bound)</t>
   </si>
   <si>
@@ -202,7 +196,25 @@
     <t>Code phức tạp</t>
   </si>
   <si>
-    <t>Cần extension</t>
+    <t>Netty / Vert.x</t>
+  </si>
+  <si>
+    <t>Event Loop + NIO</t>
+  </si>
+  <si>
+    <t>~100k–500k</t>
+  </si>
+  <si>
+    <t>Trung bình–Cao</t>
+  </si>
+  <si>
+    <t>~40–60</t>
+  </si>
+  <si>
+    <t>Ổn định, enterprise, scale tốt</t>
+  </si>
+  <si>
+    <t>JVM nặng, code verbose</t>
   </si>
 </sst>
 </file>
@@ -341,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -665,7 +677,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,7 +687,7 @@
     <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="30.5" customWidth="1"/>
     <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25" x14ac:dyDescent="0.25">
@@ -715,124 +727,124 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>39</v>
@@ -840,22 +852,22 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="25" x14ac:dyDescent="0.25">
@@ -863,19 +875,19 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="26" thickBot="1" x14ac:dyDescent="0.3">
@@ -883,19 +895,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>